<commit_message>
Aktualisierte dachser.xlsx mit neuen Tarifen
</commit_message>
<xml_diff>
--- a/dachser.xlsx
+++ b/dachser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hbecker.sharepoint.com/sites/0513_HEWI/Shared Documents/Logistik_513/Heinrich Wilke-0513 ̸ Logistik ̸ Transport ̸ Landfrachten ̸ 2024/CK/frachtenrechner 3/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hbecker.sharepoint.com/sites/0513_HEWI/Shared Documents/Logistik_513/Heinrich Wilke-0513 ̸ Logistik ̸ Transport ̸ Landfrachten ̸ 2024/CK/lkw_frachten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5AAD892B-4CCC-7147-998A-C9FEE0FC9192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB70ABB2-98A0-B645-A3F8-028DF2F2D872}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{5AAD892B-4CCC-7147-998A-C9FEE0FC9192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC6DF4E-B69A-EF44-82DC-3A03A9B0CC93}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="34560" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33400" yWindow="1240" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zonen" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4214" uniqueCount="159">
   <si>
     <t>DE</t>
   </si>
@@ -992,9 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD101"/>
+  <dimension ref="A1:AD171"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M71"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -1118,9 +1120,6 @@
       <c r="K2" t="s">
         <v>95</v>
       </c>
-      <c r="M2" t="s">
-        <v>95</v>
-      </c>
       <c r="N2" t="s">
         <v>94</v>
       </c>
@@ -1189,9 +1188,6 @@
       <c r="K3" t="s">
         <v>95</v>
       </c>
-      <c r="M3" t="s">
-        <v>95</v>
-      </c>
       <c r="N3" t="s">
         <v>94</v>
       </c>
@@ -1263,9 +1259,6 @@
       <c r="K4" t="s">
         <v>95</v>
       </c>
-      <c r="M4" t="s">
-        <v>97</v>
-      </c>
       <c r="N4" t="s">
         <v>94</v>
       </c>
@@ -1337,9 +1330,6 @@
       <c r="K5" t="s">
         <v>95</v>
       </c>
-      <c r="M5" t="s">
-        <v>97</v>
-      </c>
       <c r="N5" t="s">
         <v>94</v>
       </c>
@@ -1411,9 +1401,6 @@
       <c r="K6" t="s">
         <v>95</v>
       </c>
-      <c r="M6" t="s">
-        <v>95</v>
-      </c>
       <c r="N6" t="s">
         <v>94</v>
       </c>
@@ -1485,9 +1472,6 @@
       <c r="K7" t="s">
         <v>96</v>
       </c>
-      <c r="M7" t="s">
-        <v>96</v>
-      </c>
       <c r="N7" t="s">
         <v>94</v>
       </c>
@@ -1559,9 +1543,6 @@
       <c r="K8" t="s">
         <v>96</v>
       </c>
-      <c r="M8" t="s">
-        <v>98</v>
-      </c>
       <c r="N8" t="s">
         <v>94</v>
       </c>
@@ -1633,9 +1614,6 @@
       <c r="K9" t="s">
         <v>96</v>
       </c>
-      <c r="M9" t="s">
-        <v>97</v>
-      </c>
       <c r="N9" t="s">
         <v>94</v>
       </c>
@@ -1707,9 +1685,6 @@
       <c r="K10" t="s">
         <v>97</v>
       </c>
-      <c r="M10" t="s">
-        <v>97</v>
-      </c>
       <c r="N10" t="s">
         <v>94</v>
       </c>
@@ -1781,9 +1756,6 @@
       <c r="K11" t="s">
         <v>96</v>
       </c>
-      <c r="M11" t="s">
-        <v>94</v>
-      </c>
       <c r="N11" t="s">
         <v>94</v>
       </c>
@@ -1867,9 +1839,6 @@
       <c r="L12" t="s">
         <v>96</v>
       </c>
-      <c r="M12" t="s">
-        <v>95</v>
-      </c>
       <c r="N12" t="s">
         <v>94</v>
       </c>
@@ -1953,9 +1922,6 @@
       <c r="L13" t="s">
         <v>96</v>
       </c>
-      <c r="M13" t="s">
-        <v>95</v>
-      </c>
       <c r="N13" t="s">
         <v>94</v>
       </c>
@@ -2039,9 +2005,6 @@
       <c r="L14" t="s">
         <v>96</v>
       </c>
-      <c r="M14" t="s">
-        <v>94</v>
-      </c>
       <c r="N14" t="s">
         <v>94</v>
       </c>
@@ -2125,9 +2088,6 @@
       <c r="L15" t="s">
         <v>96</v>
       </c>
-      <c r="M15" t="s">
-        <v>95</v>
-      </c>
       <c r="N15" t="s">
         <v>94</v>
       </c>
@@ -2211,9 +2171,6 @@
       <c r="L16" t="s">
         <v>96</v>
       </c>
-      <c r="M16" t="s">
-        <v>97</v>
-      </c>
       <c r="N16" t="s">
         <v>94</v>
       </c>
@@ -2297,9 +2254,6 @@
       <c r="L17" t="s">
         <v>96</v>
       </c>
-      <c r="M17" t="s">
-        <v>97</v>
-      </c>
       <c r="N17" t="s">
         <v>95</v>
       </c>
@@ -2383,9 +2337,6 @@
       <c r="L18" t="s">
         <v>96</v>
       </c>
-      <c r="M18" t="s">
-        <v>96</v>
-      </c>
       <c r="N18" t="s">
         <v>95</v>
       </c>
@@ -2469,9 +2420,6 @@
       <c r="L19" t="s">
         <v>96</v>
       </c>
-      <c r="M19" t="s">
-        <v>96</v>
-      </c>
       <c r="N19" t="s">
         <v>95</v>
       </c>
@@ -2555,9 +2503,6 @@
       <c r="L20" t="s">
         <v>96</v>
       </c>
-      <c r="M20" t="s">
-        <v>98</v>
-      </c>
       <c r="N20" t="s">
         <v>95</v>
       </c>
@@ -2641,9 +2586,6 @@
       <c r="L21" t="s">
         <v>96</v>
       </c>
-      <c r="M21" t="s">
-        <v>94</v>
-      </c>
       <c r="N21" t="s">
         <v>95</v>
       </c>
@@ -2727,9 +2669,6 @@
       <c r="L22" t="s">
         <v>95</v>
       </c>
-      <c r="M22" t="s">
-        <v>97</v>
-      </c>
       <c r="N22" t="s">
         <v>95</v>
       </c>
@@ -2813,9 +2752,6 @@
       <c r="L23" t="s">
         <v>95</v>
       </c>
-      <c r="M23" t="s">
-        <v>96</v>
-      </c>
       <c r="N23" t="s">
         <v>95</v>
       </c>
@@ -2899,9 +2835,6 @@
       <c r="L24" t="s">
         <v>95</v>
       </c>
-      <c r="M24" t="s">
-        <v>95</v>
-      </c>
       <c r="N24" t="s">
         <v>95</v>
       </c>
@@ -2985,9 +2918,6 @@
       <c r="L25" t="s">
         <v>95</v>
       </c>
-      <c r="M25" t="s">
-        <v>95</v>
-      </c>
       <c r="N25" t="s">
         <v>96</v>
       </c>
@@ -3071,9 +3001,6 @@
       <c r="L26" t="s">
         <v>95</v>
       </c>
-      <c r="M26" t="s">
-        <v>96</v>
-      </c>
       <c r="N26" t="s">
         <v>96</v>
       </c>
@@ -3157,9 +3084,6 @@
       <c r="L27" t="s">
         <v>95</v>
       </c>
-      <c r="M27" t="s">
-        <v>96</v>
-      </c>
       <c r="N27" t="s">
         <v>96</v>
       </c>
@@ -3243,9 +3167,6 @@
       <c r="L28" t="s">
         <v>95</v>
       </c>
-      <c r="M28" t="s">
-        <v>94</v>
-      </c>
       <c r="N28" t="s">
         <v>96</v>
       </c>
@@ -3329,9 +3250,6 @@
       <c r="L29" t="s">
         <v>95</v>
       </c>
-      <c r="M29" t="s">
-        <v>95</v>
-      </c>
       <c r="N29" t="s">
         <v>95</v>
       </c>
@@ -3415,9 +3333,6 @@
       <c r="L30" t="s">
         <v>95</v>
       </c>
-      <c r="M30" t="s">
-        <v>98</v>
-      </c>
       <c r="N30" t="s">
         <v>96</v>
       </c>
@@ -3501,9 +3416,6 @@
       <c r="L31" t="s">
         <v>95</v>
       </c>
-      <c r="M31" t="s">
-        <v>94</v>
-      </c>
       <c r="N31" t="s">
         <v>96</v>
       </c>
@@ -3587,9 +3499,6 @@
       <c r="L32" t="s">
         <v>95</v>
       </c>
-      <c r="M32" t="s">
-        <v>98</v>
-      </c>
       <c r="N32" t="s">
         <v>95</v>
       </c>
@@ -3673,9 +3582,6 @@
       <c r="L33" t="s">
         <v>95</v>
       </c>
-      <c r="M33" t="s">
-        <v>97</v>
-      </c>
       <c r="N33" t="s">
         <v>95</v>
       </c>
@@ -3759,9 +3665,6 @@
       <c r="L34" t="s">
         <v>95</v>
       </c>
-      <c r="M34" t="s">
-        <v>95</v>
-      </c>
       <c r="N34" t="s">
         <v>95</v>
       </c>
@@ -3845,9 +3748,6 @@
       <c r="L35" t="s">
         <v>95</v>
       </c>
-      <c r="M35" t="s">
-        <v>95</v>
-      </c>
       <c r="N35" t="s">
         <v>95</v>
       </c>
@@ -3931,9 +3831,6 @@
       <c r="L36" t="s">
         <v>95</v>
       </c>
-      <c r="M36" t="s">
-        <v>95</v>
-      </c>
       <c r="N36" t="s">
         <v>95</v>
       </c>
@@ -4017,9 +3914,6 @@
       <c r="L37" t="s">
         <v>95</v>
       </c>
-      <c r="M37" t="s">
-        <v>95</v>
-      </c>
       <c r="N37" t="s">
         <v>95</v>
       </c>
@@ -4103,9 +3997,6 @@
       <c r="L38" t="s">
         <v>95</v>
       </c>
-      <c r="M38" t="s">
-        <v>98</v>
-      </c>
       <c r="N38" t="s">
         <v>95</v>
       </c>
@@ -4189,9 +4080,6 @@
       <c r="L39" t="s">
         <v>96</v>
       </c>
-      <c r="M39" t="s">
-        <v>98</v>
-      </c>
       <c r="N39" t="s">
         <v>95</v>
       </c>
@@ -4275,9 +4163,6 @@
       <c r="L40" t="s">
         <v>96</v>
       </c>
-      <c r="M40" t="s">
-        <v>95</v>
-      </c>
       <c r="N40" t="s">
         <v>95</v>
       </c>
@@ -4361,9 +4246,6 @@
       <c r="L41" t="s">
         <v>96</v>
       </c>
-      <c r="M41" t="s">
-        <v>97</v>
-      </c>
       <c r="N41" t="s">
         <v>95</v>
       </c>
@@ -4447,9 +4329,6 @@
       <c r="L42" t="s">
         <v>94</v>
       </c>
-      <c r="M42" t="s">
-        <v>95</v>
-      </c>
       <c r="N42" t="s">
         <v>95</v>
       </c>
@@ -4533,9 +4412,6 @@
       <c r="L43" t="s">
         <v>94</v>
       </c>
-      <c r="M43" t="s">
-        <v>94</v>
-      </c>
       <c r="N43" t="s">
         <v>95</v>
       </c>
@@ -4619,9 +4495,6 @@
       <c r="L44" t="s">
         <v>95</v>
       </c>
-      <c r="M44" t="s">
-        <v>95</v>
-      </c>
       <c r="N44" t="s">
         <v>95</v>
       </c>
@@ -4705,9 +4578,6 @@
       <c r="L45" t="s">
         <v>95</v>
       </c>
-      <c r="M45" t="s">
-        <v>95</v>
-      </c>
       <c r="N45" t="s">
         <v>95</v>
       </c>
@@ -4791,9 +4661,6 @@
       <c r="L46" t="s">
         <v>95</v>
       </c>
-      <c r="M46" t="s">
-        <v>97</v>
-      </c>
       <c r="N46" t="s">
         <v>95</v>
       </c>
@@ -4877,9 +4744,6 @@
       <c r="L47" t="s">
         <v>95</v>
       </c>
-      <c r="M47" t="s">
-        <v>95</v>
-      </c>
       <c r="N47" t="s">
         <v>95</v>
       </c>
@@ -4963,9 +4827,6 @@
       <c r="L48" t="s">
         <v>95</v>
       </c>
-      <c r="M48" t="s">
-        <v>95</v>
-      </c>
       <c r="N48" t="s">
         <v>95</v>
       </c>
@@ -5049,9 +4910,6 @@
       <c r="L49" t="s">
         <v>95</v>
       </c>
-      <c r="M49" t="s">
-        <v>94</v>
-      </c>
       <c r="N49" t="s">
         <v>95</v>
       </c>
@@ -5135,9 +4993,6 @@
       <c r="L50" t="s">
         <v>95</v>
       </c>
-      <c r="M50" t="s">
-        <v>94</v>
-      </c>
       <c r="N50" t="s">
         <v>95</v>
       </c>
@@ -5221,9 +5076,6 @@
       <c r="L51" t="s">
         <v>95</v>
       </c>
-      <c r="M51" t="s">
-        <v>97</v>
-      </c>
       <c r="N51" t="s">
         <v>95</v>
       </c>
@@ -5307,9 +5159,6 @@
       <c r="L52" t="s">
         <v>95</v>
       </c>
-      <c r="M52" t="s">
-        <v>94</v>
-      </c>
       <c r="N52" t="s">
         <v>96</v>
       </c>
@@ -5393,9 +5242,6 @@
       <c r="L53" t="s">
         <v>95</v>
       </c>
-      <c r="M53" t="s">
-        <v>95</v>
-      </c>
       <c r="N53" t="s">
         <v>96</v>
       </c>
@@ -5479,9 +5325,6 @@
       <c r="L54" t="s">
         <v>95</v>
       </c>
-      <c r="M54" t="s">
-        <v>96</v>
-      </c>
       <c r="N54" t="s">
         <v>96</v>
       </c>
@@ -5565,9 +5408,6 @@
       <c r="L55" t="s">
         <v>95</v>
       </c>
-      <c r="M55" t="s">
-        <v>94</v>
-      </c>
       <c r="N55" t="s">
         <v>96</v>
       </c>
@@ -5651,9 +5491,6 @@
       <c r="L56" t="s">
         <v>95</v>
       </c>
-      <c r="M56" t="s">
-        <v>96</v>
-      </c>
       <c r="N56" t="s">
         <v>96</v>
       </c>
@@ -5737,9 +5574,6 @@
       <c r="L57" t="s">
         <v>95</v>
       </c>
-      <c r="M57" t="s">
-        <v>96</v>
-      </c>
       <c r="N57" t="s">
         <v>96</v>
       </c>
@@ -5823,9 +5657,6 @@
       <c r="L58" t="s">
         <v>95</v>
       </c>
-      <c r="M58" t="s">
-        <v>94</v>
-      </c>
       <c r="N58" t="s">
         <v>96</v>
       </c>
@@ -5909,9 +5740,6 @@
       <c r="L59" t="s">
         <v>95</v>
       </c>
-      <c r="M59" t="s">
-        <v>97</v>
-      </c>
       <c r="N59" t="s">
         <v>96</v>
       </c>
@@ -5995,9 +5823,6 @@
       <c r="L60" t="s">
         <v>95</v>
       </c>
-      <c r="M60" t="s">
-        <v>96</v>
-      </c>
       <c r="N60" t="s">
         <v>96</v>
       </c>
@@ -6081,9 +5906,6 @@
       <c r="L61" t="s">
         <v>95</v>
       </c>
-      <c r="M61" t="s">
-        <v>95</v>
-      </c>
       <c r="N61" t="s">
         <v>96</v>
       </c>
@@ -6167,9 +5989,6 @@
       <c r="L62" t="s">
         <v>95</v>
       </c>
-      <c r="M62" t="s">
-        <v>94</v>
-      </c>
       <c r="N62" t="s">
         <v>96</v>
       </c>
@@ -6253,9 +6072,6 @@
       <c r="L63" t="s">
         <v>95</v>
       </c>
-      <c r="M63" t="s">
-        <v>94</v>
-      </c>
       <c r="N63" t="s">
         <v>96</v>
       </c>
@@ -6339,9 +6155,6 @@
       <c r="L64" t="s">
         <v>95</v>
       </c>
-      <c r="M64" t="s">
-        <v>97</v>
-      </c>
       <c r="N64" t="s">
         <v>96</v>
       </c>
@@ -6425,9 +6238,6 @@
       <c r="L65" t="s">
         <v>95</v>
       </c>
-      <c r="M65" t="s">
-        <v>94</v>
-      </c>
       <c r="N65" t="s">
         <v>96</v>
       </c>
@@ -6511,9 +6321,6 @@
       <c r="L66" t="s">
         <v>95</v>
       </c>
-      <c r="M66" t="s">
-        <v>96</v>
-      </c>
       <c r="N66" t="s">
         <v>96</v>
       </c>
@@ -6597,9 +6404,6 @@
       <c r="L67" t="s">
         <v>96</v>
       </c>
-      <c r="M67" t="s">
-        <v>97</v>
-      </c>
       <c r="N67" t="s">
         <v>97</v>
       </c>
@@ -6683,9 +6487,6 @@
       <c r="L68" t="s">
         <v>96</v>
       </c>
-      <c r="M68" t="s">
-        <v>96</v>
-      </c>
       <c r="N68" t="s">
         <v>97</v>
       </c>
@@ -6769,9 +6570,6 @@
       <c r="L69" t="s">
         <v>96</v>
       </c>
-      <c r="M69" t="s">
-        <v>96</v>
-      </c>
       <c r="N69" t="s">
         <v>96</v>
       </c>
@@ -6855,9 +6653,6 @@
       <c r="L70" t="s">
         <v>96</v>
       </c>
-      <c r="M70" t="s">
-        <v>97</v>
-      </c>
       <c r="N70" t="s">
         <v>96</v>
       </c>
@@ -6941,9 +6736,6 @@
       <c r="L71" t="s">
         <v>96</v>
       </c>
-      <c r="M71" t="s">
-        <v>97</v>
-      </c>
       <c r="N71" t="s">
         <v>96</v>
       </c>
@@ -9388,6 +9180,566 @@
       </c>
       <c r="AD101" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30">
+      <c r="A102" t="s">
+        <v>28</v>
+      </c>
+      <c r="M102" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30">
+      <c r="A103" t="s">
+        <v>29</v>
+      </c>
+      <c r="M103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:30">
+      <c r="A104" t="s">
+        <v>30</v>
+      </c>
+      <c r="M104" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:30">
+      <c r="A105" t="s">
+        <v>31</v>
+      </c>
+      <c r="M105" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="1:30">
+      <c r="A106" t="s">
+        <v>32</v>
+      </c>
+      <c r="M106" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:30">
+      <c r="A107" t="s">
+        <v>33</v>
+      </c>
+      <c r="M107" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30">
+      <c r="A108" t="s">
+        <v>34</v>
+      </c>
+      <c r="M108" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30">
+      <c r="A109" t="s">
+        <v>35</v>
+      </c>
+      <c r="M109" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="M110" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+      <c r="M111" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30">
+      <c r="A112" t="s">
+        <v>37</v>
+      </c>
+      <c r="M112" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
+      <c r="A113" t="s">
+        <v>38</v>
+      </c>
+      <c r="M113" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
+      <c r="A114" t="s">
+        <v>39</v>
+      </c>
+      <c r="M114" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
+      <c r="A115" t="s">
+        <v>0</v>
+      </c>
+      <c r="M115" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
+      <c r="A116" t="s">
+        <v>40</v>
+      </c>
+      <c r="M116" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
+      <c r="A117" t="s">
+        <v>41</v>
+      </c>
+      <c r="M117" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
+      <c r="A118" t="s">
+        <v>42</v>
+      </c>
+      <c r="M118" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="A119" t="s">
+        <v>43</v>
+      </c>
+      <c r="M119" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
+      <c r="A120" t="s">
+        <v>44</v>
+      </c>
+      <c r="M120" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
+      <c r="A121" t="s">
+        <v>45</v>
+      </c>
+      <c r="M121" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
+      <c r="A122" t="s">
+        <v>46</v>
+      </c>
+      <c r="M122" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
+      <c r="A123" t="s">
+        <v>47</v>
+      </c>
+      <c r="M123" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13">
+      <c r="A124" t="s">
+        <v>48</v>
+      </c>
+      <c r="M124" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
+      <c r="A125" t="s">
+        <v>49</v>
+      </c>
+      <c r="M125" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
+      <c r="A126" t="s">
+        <v>18</v>
+      </c>
+      <c r="M126" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
+      <c r="A127" t="s">
+        <v>50</v>
+      </c>
+      <c r="M127" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" t="s">
+        <v>51</v>
+      </c>
+      <c r="M128" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
+      <c r="A129" t="s">
+        <v>52</v>
+      </c>
+      <c r="M129" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
+      <c r="A130" t="s">
+        <v>53</v>
+      </c>
+      <c r="M130" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
+      <c r="A131" t="s">
+        <v>54</v>
+      </c>
+      <c r="M131" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
+      <c r="A132" t="s">
+        <v>55</v>
+      </c>
+      <c r="M132" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133" t="s">
+        <v>56</v>
+      </c>
+      <c r="M133" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
+      <c r="A134" t="s">
+        <v>57</v>
+      </c>
+      <c r="M134" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
+      <c r="A135" t="s">
+        <v>58</v>
+      </c>
+      <c r="M135" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
+      <c r="A136" t="s">
+        <v>59</v>
+      </c>
+      <c r="M136" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
+      <c r="A137" t="s">
+        <v>60</v>
+      </c>
+      <c r="M137" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
+      <c r="A138" t="s">
+        <v>61</v>
+      </c>
+      <c r="M138" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
+      <c r="A139" t="s">
+        <v>62</v>
+      </c>
+      <c r="M139" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
+      <c r="A140" t="s">
+        <v>63</v>
+      </c>
+      <c r="M140" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
+      <c r="A141" t="s">
+        <v>64</v>
+      </c>
+      <c r="M141" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
+      <c r="A142" t="s">
+        <v>65</v>
+      </c>
+      <c r="M142" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
+      <c r="A143" t="s">
+        <v>66</v>
+      </c>
+      <c r="M143" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
+      <c r="A144" t="s">
+        <v>67</v>
+      </c>
+      <c r="M144" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
+      <c r="A145" t="s">
+        <v>68</v>
+      </c>
+      <c r="M145" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
+      <c r="A146" t="s">
+        <v>69</v>
+      </c>
+      <c r="M146" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
+      <c r="A147" t="s">
+        <v>70</v>
+      </c>
+      <c r="M147" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
+      <c r="A148" t="s">
+        <v>71</v>
+      </c>
+      <c r="M148" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
+      <c r="A149" t="s">
+        <v>72</v>
+      </c>
+      <c r="M149" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
+      <c r="A150" t="s">
+        <v>73</v>
+      </c>
+      <c r="M150" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
+      <c r="A151" t="s">
+        <v>74</v>
+      </c>
+      <c r="M151" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
+      <c r="A152" t="s">
+        <v>25</v>
+      </c>
+      <c r="M152" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
+      <c r="A153" t="s">
+        <v>75</v>
+      </c>
+      <c r="M153" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
+      <c r="A154" t="s">
+        <v>26</v>
+      </c>
+      <c r="M154" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13">
+      <c r="A155" t="s">
+        <v>76</v>
+      </c>
+      <c r="M155" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
+      <c r="A156" t="s">
+        <v>77</v>
+      </c>
+      <c r="M156" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
+      <c r="A157" t="s">
+        <v>78</v>
+      </c>
+      <c r="M157" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
+      <c r="A158" t="s">
+        <v>79</v>
+      </c>
+      <c r="M158" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
+      <c r="A159" t="s">
+        <v>80</v>
+      </c>
+      <c r="M159" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13">
+      <c r="A160" t="s">
+        <v>81</v>
+      </c>
+      <c r="M160" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13">
+      <c r="A161" t="s">
+        <v>82</v>
+      </c>
+      <c r="M161" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13">
+      <c r="A162" t="s">
+        <v>83</v>
+      </c>
+      <c r="M162" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13">
+      <c r="A163" t="s">
+        <v>84</v>
+      </c>
+      <c r="M163" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13">
+      <c r="A164" t="s">
+        <v>85</v>
+      </c>
+      <c r="M164" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13">
+      <c r="A165" t="s">
+        <v>86</v>
+      </c>
+      <c r="M165" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13">
+      <c r="A166" t="s">
+        <v>87</v>
+      </c>
+      <c r="M166" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13">
+      <c r="A167" t="s">
+        <v>88</v>
+      </c>
+      <c r="M167" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13">
+      <c r="A168" t="s">
+        <v>89</v>
+      </c>
+      <c r="M168" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13">
+      <c r="A169" t="s">
+        <v>90</v>
+      </c>
+      <c r="M169" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13">
+      <c r="A170" t="s">
+        <v>91</v>
+      </c>
+      <c r="M170" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13">
+      <c r="A171" t="s">
+        <v>92</v>
+      </c>
+      <c r="M171" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -13552,7 +13904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33496B4-D06E-1A45-93B2-FADD1BFC37A2}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F35"/>
     </sheetView>
   </sheetViews>

</xml_diff>